<commit_message>
fixed a minor bug in function sln_results.createTable
there is a random '+' in one of the file path
</commit_message>
<xml_diff>
--- a/result_table_templates/AverageOptoSingleVC.xlsx
+++ b/result_table_templates/AverageOptoSingleVC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming\githubRepos\DJ_schwartzlab\result_table_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD0518D-B28F-44E5-A8C5-0137CCDD0CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC08350-4696-42D6-BB77-FE28887495A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2215" yWindow="2245" windowWidth="14400" windowHeight="8250" xr2:uid="{000E7EE4-D028-4B0A-AFBF-C8FD792C3CE0}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{000E7EE4-D028-4B0A-AFBF-C8FD792C3CE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Field</t>
   </si>
@@ -65,9 +65,6 @@
     <t>source_id</t>
   </si>
   <si>
-    <t>unit 16</t>
-  </si>
-  <si>
     <t>source id used to identify the cell to which the dataset belongs</t>
   </si>
   <si>
@@ -98,13 +95,13 @@
     <t>the average trace of the dataset</t>
   </si>
   <si>
-    <t>blob</t>
-  </si>
-  <si>
     <t>sample_rate</t>
   </si>
   <si>
     <t>the rate of electrode sampling signals</t>
+  </si>
+  <si>
+    <t>cell</t>
   </si>
 </sst>
 </file>
@@ -479,7 +476,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -525,68 +522,71 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
         <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
         <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" display="blob@raw" xr:uid="{28FD44DE-697F-41D1-9CC1-6F8812C8043F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added table for sln_results for opto
new table AverageOptoSingleVC for making a baseline subtracted average trace for voltage clamp/optopulse protocol
</commit_message>
<xml_diff>
--- a/result_table_templates/AverageOptoSingleVC.xlsx
+++ b/result_table_templates/AverageOptoSingleVC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming\githubRepos\DJ_schwartzlab\result_table_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC08350-4696-42D6-BB77-FE28887495A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B65A4A-56C9-496E-87DC-2D4BA09959B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{000E7EE4-D028-4B0A-AFBF-C8FD792C3CE0}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{000E7EE4-D028-4B0A-AFBF-C8FD792C3CE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Field</t>
   </si>
@@ -93,12 +93,6 @@
   </si>
   <si>
     <t>the average trace of the dataset</t>
-  </si>
-  <si>
-    <t>sample_rate</t>
-  </si>
-  <si>
-    <t>the rate of electrode sampling signals</t>
   </si>
   <si>
     <t>cell</t>
@@ -473,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{241D372B-DFAD-4515-91F3-7BE2FC61061E}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -566,21 +560,10 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing minor bugs in average trace VC opto
</commit_message>
<xml_diff>
--- a/result_table_templates/AverageOptoSingleVC.xlsx
+++ b/result_table_templates/AverageOptoSingleVC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming\githubRepos\DJ_schwartzlab\result_table_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B65A4A-56C9-496E-87DC-2D4BA09959B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FAE9C1-7DAE-4F64-B1A6-C1AAB4789C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{000E7EE4-D028-4B0A-AFBF-C8FD792C3CE0}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{000E7EE4-D028-4B0A-AFBF-C8FD792C3CE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Field</t>
   </si>
@@ -96,6 +96,18 @@
   </si>
   <si>
     <t>cell</t>
+  </si>
+  <si>
+    <t>sample_rate</t>
+  </si>
+  <si>
+    <t>sampling rate of the recording</t>
+  </si>
+  <si>
+    <t>epoch_total</t>
+  </si>
+  <si>
+    <t>the total number of the epochs</t>
   </si>
 </sst>
 </file>
@@ -467,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{241D372B-DFAD-4515-91F3-7BE2FC61061E}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -566,6 +578,28 @@
         <v>18</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" display="blob@raw" xr:uid="{28FD44DE-697F-41D1-9CC1-6F8812C8043F}"/>

</xml_diff>

<commit_message>
Update for synaptic detection analysis
1. added a new table sln_results.EpochPostsynapticCurrent
2. filled up DJ analysis table creation function where case 'Epoch' was blank and no primary or secondary keys were set based on the input
3. included a modified version of MATLAB open source script detectPSP for voltage clamp recording
</commit_message>
<xml_diff>
--- a/result_table_templates/AverageOptoSingleVC.xlsx
+++ b/result_table_templates/AverageOptoSingleVC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming\githubRepos\DJ_schwartzlab\result_table_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FAE9C1-7DAE-4F64-B1A6-C1AAB4789C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCF884B-B691-4535-9DA2-D9E53930FA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{000E7EE4-D028-4B0A-AFBF-C8FD792C3CE0}"/>
   </bookViews>
@@ -482,7 +482,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>

</xml_diff>